<commit_message>
Update labels by Mahdi
</commit_message>
<xml_diff>
--- a/tools/labels.xlsx
+++ b/tools/labels.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1179" uniqueCount="592">
   <si>
     <t xml:space="preserve">images</t>
   </si>
@@ -1838,7 +1838,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1173">
+  <borders count="1185">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1846,6 +1846,18 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
     <border/>
     <border/>
     <border/>
@@ -3048,7 +3060,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1178">
+  <cellXfs count="1190">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4245,6 +4257,18 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1170" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1171" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1172" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1173" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1174" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1175" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1176" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1177" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1178" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1179" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1180" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1181" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1182" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1183" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1184" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4302,8 +4326,8 @@
         <v>2</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" s="8" t="s">
-        <v>588</v>
+      <c r="C2" s="1178" t="s">
+        <v>589</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -4362,8 +4386,8 @@
         <v>6</v>
       </c>
       <c r="B6" s="1"/>
-      <c r="C6" s="16" t="s">
-        <v>590</v>
+      <c r="C6" s="1180" t="s">
+        <v>589</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -4480,8 +4504,8 @@
         <v>16</v>
       </c>
       <c r="B16" s="1"/>
-      <c r="C16" s="36" t="s">
-        <v>589</v>
+      <c r="C16" s="1182" t="s">
+        <v>588</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -4502,8 +4526,8 @@
         <v>18</v>
       </c>
       <c r="B18" s="1"/>
-      <c r="C18" s="40" t="s">
-        <v>589</v>
+      <c r="C18" s="1184" t="s">
+        <v>588</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -5085,8 +5109,8 @@
         <v>71</v>
       </c>
       <c r="B71" s="1"/>
-      <c r="C71" s="146" t="s">
-        <v>591</v>
+      <c r="C71" s="1186" t="s">
+        <v>589</v>
       </c>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
@@ -5129,8 +5153,8 @@
         <v>75</v>
       </c>
       <c r="B75" s="1"/>
-      <c r="C75" s="154" t="s">
-        <v>589</v>
+      <c r="C75" s="1188" t="s">
+        <v>588</v>
       </c>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>

</xml_diff>